<commit_message>
Some database tests added.
</commit_message>
<xml_diff>
--- a/src/test/resources/masterTest.xlsx
+++ b/src/test/resources/masterTest.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14955" windowHeight="5880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Code</t>
   </si>
@@ -34,12 +35,15 @@
   </si>
   <si>
     <t>Sensor</t>
+  </si>
+  <si>
+    <t>Company</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -350,11 +354,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -391,6 +395,14 @@
         <v>4</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>